<commit_message>
complete lab1 AOM and add lectures
</commit_message>
<xml_diff>
--- a/Applied_Optimization_Models/Lab_Limenitiz/lab1/ЛР1.xlsx
+++ b/Applied_Optimization_Models/Lab_Limenitiz/lab1/ЛР1.xlsx
@@ -5,47 +5,51 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Projects\SUAI\ПМО\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Projects\SUAI\Applied_Optimization_Models\Lab_Limenitiz\lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F29439E-5F25-4AD4-A6CE-C8CB6E97D206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670E9B81-76A5-49DC-B31F-899FDA32135B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AD0720CC-D704-4E02-B865-9941600603DD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{AD0720CC-D704-4E02-B865-9941600603DD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Отчет о результатах 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Отчет об устойчивости 1" sheetId="3" r:id="rId2"/>
+    <sheet name="Отчет о пределах 1" sheetId="4" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Лист1!$B$14:$C$14</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Лист1!$D$6:$D$7</definedName>
-    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Лист1!$D$9</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Лист1!$F$6:$F$7</definedName>
-    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">Лист1!$B$16:$C$16</definedName>
+    <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">Лист1!$D$6:$D$7</definedName>
+    <definedName name="solver_mip" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">Лист1!$D$9</definedName>
+    <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">Лист1!$F$6:$F$7</definedName>
+    <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="3" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -57,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
   <si>
     <t>Время</t>
   </si>
@@ -93,13 +97,184 @@
   </si>
   <si>
     <t xml:space="preserve">Объем производства </t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Отчет о результатах</t>
+  </si>
+  <si>
+    <t>Лист: [ЛР1.xlsx]Лист1</t>
+  </si>
+  <si>
+    <t>Отчет создан: 23.09.2021 1:07:10</t>
+  </si>
+  <si>
+    <t>Результат: Решение найдено. Все ограничения и условия оптимальности выполнены.</t>
+  </si>
+  <si>
+    <t>Модуль поиска решения</t>
+  </si>
+  <si>
+    <t>Модуль: Поиск решения лин. задач симплекс-методом</t>
+  </si>
+  <si>
+    <t>Время решения: 0,032 секунд.</t>
+  </si>
+  <si>
+    <t>Число итераций: 3 Число подзадач: 0</t>
+  </si>
+  <si>
+    <t>Параметры поиска решения</t>
+  </si>
+  <si>
+    <t>Максимальное время Без пределов,  Число итераций Без пределов, Precision 0,000001</t>
+  </si>
+  <si>
+    <t>Максимальное число подзадач Без пределов, Максимальное число целочисленных решений Без пределов, Целочисленное отклонение 1%, Считать неотрицательными</t>
+  </si>
+  <si>
+    <t>Ячейка целевой функции (Максимум)</t>
+  </si>
+  <si>
+    <t>Ячейка</t>
+  </si>
+  <si>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>Исходное значение</t>
+  </si>
+  <si>
+    <t>Окончательное значение</t>
+  </si>
+  <si>
+    <t>Ячейки переменных</t>
+  </si>
+  <si>
+    <t>Целочисленное</t>
+  </si>
+  <si>
+    <t>Ограничения</t>
+  </si>
+  <si>
+    <t>Значение ячейки</t>
+  </si>
+  <si>
+    <t>Формула</t>
+  </si>
+  <si>
+    <t>Состояние</t>
+  </si>
+  <si>
+    <t>Допуск</t>
+  </si>
+  <si>
+    <t>$D$9</t>
+  </si>
+  <si>
+    <t>Доход Суммарная прибыль</t>
+  </si>
+  <si>
+    <t>$B$16</t>
+  </si>
+  <si>
+    <t>Объем производства  Тип напитка</t>
+  </si>
+  <si>
+    <t>Продолжить</t>
+  </si>
+  <si>
+    <t>$C$16</t>
+  </si>
+  <si>
+    <t>$D$6</t>
+  </si>
+  <si>
+    <t>Время Всего затрачено</t>
+  </si>
+  <si>
+    <t>$D$6&lt;=$F$6</t>
+  </si>
+  <si>
+    <t>Привязка</t>
+  </si>
+  <si>
+    <t>$D$7</t>
+  </si>
+  <si>
+    <t>Ингридиенты Всего затрачено</t>
+  </si>
+  <si>
+    <t>$D$7&lt;=$F$7</t>
+  </si>
+  <si>
+    <t>Без привязки</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Отчет об устойчивости</t>
+  </si>
+  <si>
+    <t>Окончательное</t>
+  </si>
+  <si>
+    <t>Значение</t>
+  </si>
+  <si>
+    <t>Приведенн.</t>
+  </si>
+  <si>
+    <t>Стоимость</t>
+  </si>
+  <si>
+    <t>Целевая функция</t>
+  </si>
+  <si>
+    <t>Коэффициент</t>
+  </si>
+  <si>
+    <t>Допустимое</t>
+  </si>
+  <si>
+    <t>Увеличение</t>
+  </si>
+  <si>
+    <t>Уменьшение</t>
+  </si>
+  <si>
+    <t>Тень</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>Ограничение</t>
+  </si>
+  <si>
+    <t>Правая сторона</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Отчет о пределах</t>
+  </si>
+  <si>
+    <t>Переменная</t>
+  </si>
+  <si>
+    <t>Нижний</t>
+  </si>
+  <si>
+    <t>Предел</t>
+  </si>
+  <si>
+    <t>Результат</t>
+  </si>
+  <si>
+    <t>Верхний</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +286,24 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -137,11 +330,60 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -151,13 +393,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% — акцент1" xfId="1" builtinId="30"/>
@@ -473,21 +729,640 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E64673-40AA-4564-822C-1C3B3A85E842}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="8">
+        <v>300</v>
+      </c>
+      <c r="E16" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1200</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1200</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="9">
+        <v>24</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G27" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="8">
+        <v>12</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" s="5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58755909-B695-4E83-A6E9-910CDF9071DB}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1200</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1E+30</v>
+      </c>
+      <c r="H9" s="7">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>-0.14999999999999997</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.35</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.14999999999999997</v>
+      </c>
+      <c r="H10" s="5">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="7">
+        <v>24</v>
+      </c>
+      <c r="E15" s="7">
+        <v>12.500000000000002</v>
+      </c>
+      <c r="F15" s="7">
+        <v>24</v>
+      </c>
+      <c r="G15" s="7">
+        <v>8</v>
+      </c>
+      <c r="H15" s="7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="5">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>16</v>
+      </c>
+      <c r="G16" s="5">
+        <v>1E+30</v>
+      </c>
+      <c r="H16" s="5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E086F725-608A-427E-8DDE-9D7BAAA1AE17}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="10"/>
+      <c r="F11" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="9">
+        <v>1200</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9">
+        <v>1200</v>
+      </c>
+      <c r="J13" s="9">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>300</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0</v>
+      </c>
+      <c r="J14" s="8">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAC74783-DBD0-4ADA-8596-D0A4744A0294}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.21875" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5546875" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -507,10 +1382,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="3"/>
       <c r="D4" t="s">
         <v>6</v>
       </c>
@@ -533,20 +1408,20 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.02</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.04</v>
       </c>
       <c r="D6">
-        <f>SUMPRODUCT(B6:C6,B14:C14)</f>
-        <v>23.999999999999993</v>
+        <f>SUMPRODUCT(B6:C6,B16:C16)</f>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>24</v>
       </c>
     </row>
@@ -554,20 +1429,20 @@
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.01</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.04</v>
       </c>
       <c r="D7">
-        <f>SUMPRODUCT(B7:C7,B14:C14)</f>
-        <v>11.999999999999996</v>
+        <f>SUMPRODUCT(B7:C7,B16:C16)</f>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>16</v>
       </c>
     </row>
@@ -580,51 +1455,51 @@
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>0.25</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>0.35</v>
       </c>
       <c r="D9">
-        <f>SUMPRODUCT(B9:C9,B14:C14)</f>
-        <v>299.99999999999989</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+        <f>SUMPRODUCT(B9:C9,B16:C16)</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="1" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B13">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B15">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C15">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="3">
-        <v>1199.9999999999995</v>
-      </c>
-      <c r="C14" s="3">
+      <c r="B16" s="2">
+        <v>1200</v>
+      </c>
+      <c r="C16" s="2">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>